<commit_message>
Federated IDM overview updates.
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -4,24 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
-    <sheet name="SSO" sheetId="1" r:id="rId1"/>
+    <sheet name="SSOProtocols" sheetId="1" r:id="rId1"/>
     <sheet name="Vertinimas" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
-  <si>
-    <t>Saugumo rizikos</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>Yra</t>
   </si>
@@ -35,12 +29,6 @@
     <t>Naudotojo sutikimas perduoti duomenis</t>
   </si>
   <si>
-    <t>Šifravimas</t>
-  </si>
-  <si>
-    <t>Pasirašymas</t>
-  </si>
-  <si>
     <t>JSON, JWT</t>
   </si>
   <si>
@@ -50,12 +38,6 @@
     <t>Duomenų formatas</t>
   </si>
   <si>
-    <t>HTTP</t>
-  </si>
-  <si>
-    <t>SAML, HTTP</t>
-  </si>
-  <si>
     <t>Duomenų perdavimas</t>
   </si>
   <si>
@@ -92,7 +74,34 @@
     <t>SAML</t>
   </si>
   <si>
-    <t>Savybė</t>
+    <t>HTTP, REST</t>
+  </si>
+  <si>
+    <t>HTTP, SOAP</t>
+  </si>
+  <si>
+    <t>Duomenų šifravimas</t>
+  </si>
+  <si>
+    <t>Viešo-privataus rakto infrastruktūra</t>
+  </si>
+  <si>
+    <t>Neapibrėžta (palikta realizacijai)</t>
+  </si>
+  <si>
+    <t>Tapatybės tiekėjo suteiktų duomenų validavimas</t>
+  </si>
+  <si>
+    <t>Naudojančios organizacijos</t>
+  </si>
+  <si>
+    <t>Google, Microsoft, Ping Identity</t>
+  </si>
+  <si>
+    <t>Google, Amazon, GitHub</t>
+  </si>
+  <si>
+    <t>Salesforce, PingFederate, Oracle Access Manager</t>
   </si>
 </sst>
 </file>
@@ -166,23 +175,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Universitetų reitingai"/>
-      <sheetName val="Excel2LaTeX"/>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -474,139 +466,155 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21.21875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.21875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -618,7 +626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>

<commit_message>
IDM comparison and main federated IDM problems
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SSOProtocols" sheetId="1" r:id="rId1"/>
-    <sheet name="Vertinimas" sheetId="2" r:id="rId2"/>
+    <sheet name="IDMEvaluation" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="65">
   <si>
     <t>Yra</t>
   </si>
@@ -102,14 +102,151 @@
   </si>
   <si>
     <t>Salesforce, PingFederate, Oracle Access Manager</t>
+  </si>
+  <si>
+    <t>Patogumas</t>
+  </si>
+  <si>
+    <t>Atpažinimo duomenys</t>
+  </si>
+  <si>
+    <t>Saugumas</t>
+  </si>
+  <si>
+    <t>Technologiniai standartai</t>
+  </si>
+  <si>
+    <t>Kontrolė</t>
+  </si>
+  <si>
+    <t>Vienas nesėkmės taškas</t>
+  </si>
+  <si>
+    <t>Trust!</t>
+  </si>
+  <si>
+    <t>Izoliuotas</t>
+  </si>
+  <si>
+    <t>Centralizuotas</t>
+  </si>
+  <si>
+    <t>Jungtinis</t>
+  </si>
+  <si>
+    <t>Kiekvienai paslaugai</t>
+  </si>
+  <si>
+    <t>Kiekvienam paslaugos tiekėjui</t>
+  </si>
+  <si>
+    <t>Kiekvienam tapatybės tiekėjui</t>
+  </si>
+  <si>
+    <t>Tiek, kiek tapatybės tiekėjų</t>
+  </si>
+  <si>
+    <t>Tiek, kiek paslaugų</t>
+  </si>
+  <si>
+    <t>Prisijungimų kiekis</t>
+  </si>
+  <si>
+    <t>Tiek, kiek paslaugų tiekėjų</t>
+  </si>
+  <si>
+    <t>Galimi</t>
+  </si>
+  <si>
+    <t>Paslaugų tiekėjo tapatybės valdymo modulis</t>
+  </si>
+  <si>
+    <t>Tapatybės tiekėjas</t>
+  </si>
+  <si>
+    <t>Paslaugų tiekėjo nuožiūra</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Nukreipimai (angl. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>redirects)</t>
+    </r>
+  </si>
+  <si>
+    <t>Paslaugos kūrėjo nuožiūra</t>
+  </si>
+  <si>
+    <t>SAML 2.0, OAuth 2.0, OpenID Connect</t>
+  </si>
+  <si>
+    <t>Naudotojo patvirtinimas duomenis perduodant kitai paslaugai</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Tai realizavus paslaugų tiekėjui</t>
+  </si>
+  <si>
+    <t>Tai realizavus paslaugos kūrėjui</t>
+  </si>
+  <si>
+    <t>Naudotojo patirties vientisumas</t>
+  </si>
+  <si>
+    <t>Duomenų suteikimas tik jų prireikus</t>
+  </si>
+  <si>
+    <t>Galimas (OAuth 2.0, OpenID Connect)</t>
+  </si>
+  <si>
+    <t>Dalinis (dar nenaudotam paslaugų tiekėjui prašant naudotojo patvirtinimo)</t>
+  </si>
+  <si>
+    <t>Tapatybės duomenų keitimas</t>
+  </si>
+  <si>
+    <t>Kiekvieno tapatybės tiekėjo tinklalapyje</t>
+  </si>
+  <si>
+    <t>Kiekvieno paslaugų tiekėjo tinklalapyje</t>
+  </si>
+  <si>
+    <t>Kiekvienos paslaugos tinklalapyje</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -125,7 +262,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -148,17 +285,194 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -466,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -480,13 +794,13 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -624,12 +938,183 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="13.21875" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.21875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="22.109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="16.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" s="4" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="20"/>
+      <c r="C2" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+    </row>
+    <row r="3" spans="2:11" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="21"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B4" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B5" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B6" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C11" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:K2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Start of blockchainIDM model + structure of sections
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView minimized="1" xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="SSOProtocols" sheetId="1" r:id="rId1"/>
     <sheet name="IDMEvaluation" sheetId="2" r:id="rId2"/>
+    <sheet name="BlockchainComparison" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="79">
   <si>
     <t>Yra</t>
   </si>
@@ -207,6 +208,51 @@
   </si>
   <si>
     <t>Dalinis (dar nenaudotai paslaugai prašant naudotojo patvirtinimo)</t>
+  </si>
+  <si>
+    <t>Vieša</t>
+  </si>
+  <si>
+    <t>Privati</t>
+  </si>
+  <si>
+    <t>Konsorciumo</t>
+  </si>
+  <si>
+    <t>Visi kasėjai</t>
+  </si>
+  <si>
+    <t>Išrinkti tinklo dalyviai</t>
+  </si>
+  <si>
+    <t>Viena organizacija</t>
+  </si>
+  <si>
+    <t>Skaitymo teisės</t>
+  </si>
+  <si>
+    <t>Viešos</t>
+  </si>
+  <si>
+    <t>Gali būti viešos ar apribotos</t>
+  </si>
+  <si>
+    <t>Efektyvumas</t>
+  </si>
+  <si>
+    <t>Mažas</t>
+  </si>
+  <si>
+    <t>Didelis</t>
+  </si>
+  <si>
+    <t>Centralizuotumas</t>
+  </si>
+  <si>
+    <t>Dalinis</t>
+  </si>
+  <si>
+    <t>Konsensuso nustatymas</t>
   </si>
 </sst>
 </file>
@@ -265,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -283,21 +329,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,7 +652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -764,7 +812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
@@ -780,15 +828,15 @@
       <c r="C1" s="4"/>
     </row>
     <row r="2" spans="3:10" s="6" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="9" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>38</v>
       </c>
       <c r="H2" s="5"/>
@@ -796,25 +844,25 @@
       <c r="J2" s="5"/>
     </row>
     <row r="3" spans="3:10" s="2" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11" t="s">
+      <c r="D3" s="11"/>
+      <c r="E3" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="9" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="4" spans="3:10" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="9" t="s">
         <v>43</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -831,8 +879,8 @@
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C5" s="7"/>
-      <c r="D5" s="8" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="7" t="s">
         <v>55</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -849,10 +897,10 @@
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>31</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -869,8 +917,8 @@
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="3:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C7" s="7"/>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="7" t="s">
         <v>35</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -887,8 +935,8 @@
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C8" s="7"/>
-      <c r="D8" s="8" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="7" t="s">
         <v>33</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -905,10 +953,10 @@
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="3:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -925,8 +973,8 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="3:10" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="7"/>
-      <c r="D10" s="8" t="s">
+      <c r="C10" s="10"/>
+      <c r="D10" s="7" t="s">
         <v>56</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -943,8 +991,8 @@
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="3:10" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="7"/>
-      <c r="D11" s="8" t="s">
+      <c r="C11" s="10"/>
+      <c r="D11" s="7" t="s">
         <v>57</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -970,4 +1018,94 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="17" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="4" max="4" width="21.21875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="1"/>
+      <c r="C2" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Two-level deep TOC. Fixes after review with Aurimas.
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SSOProtocols" sheetId="1" r:id="rId1"/>
     <sheet name="IDMEvaluation" sheetId="2" r:id="rId2"/>
     <sheet name="BlockchainComparison" sheetId="3" r:id="rId3"/>
+    <sheet name="SmartContractPrices" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="91">
   <si>
     <t>Yra</t>
   </si>
@@ -253,13 +254,49 @@
   </si>
   <si>
     <t>Konsensuso nustatymas</t>
+  </si>
+  <si>
+    <t>Kuras</t>
+  </si>
+  <si>
+    <t>Kaina, ETH</t>
+  </si>
+  <si>
+    <t>Kaina, €</t>
+  </si>
+  <si>
+    <t>Vienetas</t>
+  </si>
+  <si>
+    <t>Funkcija getAttributeAsUser</t>
+  </si>
+  <si>
+    <t>Funkcija getAttribute</t>
+  </si>
+  <si>
+    <t>Funkcija removeAccess</t>
+  </si>
+  <si>
+    <t>Funkcija grantAccess</t>
+  </si>
+  <si>
+    <t>Funkcija requestAttributeAccess</t>
+  </si>
+  <si>
+    <t>Kontrakto sukūrimas</t>
+  </si>
+  <si>
+    <t>Saugomas string "tZM11CdI7z4mZJc+/5kg3Q=="</t>
+  </si>
+  <si>
+    <t>Kuris yra "+37063554865"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,16 +312,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF73879C"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -307,11 +356,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -338,14 +402,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,7 +721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -828,8 +897,8 @@
       <c r="C1" s="4"/>
     </row>
     <row r="2" spans="3:10" s="6" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
       <c r="E2" s="8" t="s">
         <v>36</v>
       </c>
@@ -844,10 +913,10 @@
       <c r="J2" s="5"/>
     </row>
     <row r="3" spans="3:10" s="2" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="11"/>
+      <c r="D3" s="13"/>
       <c r="E3" s="9" t="s">
         <v>39</v>
       </c>
@@ -859,7 +928,7 @@
       </c>
     </row>
     <row r="4" spans="3:10" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="12" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="9" t="s">
@@ -879,7 +948,7 @@
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C5" s="10"/>
+      <c r="C5" s="12"/>
       <c r="D5" s="7" t="s">
         <v>55</v>
       </c>
@@ -897,7 +966,7 @@
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="12" t="s">
         <v>32</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -917,7 +986,7 @@
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="3:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C7" s="10"/>
+      <c r="C7" s="12"/>
       <c r="D7" s="7" t="s">
         <v>35</v>
       </c>
@@ -935,7 +1004,7 @@
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C8" s="10"/>
+      <c r="C8" s="12"/>
       <c r="D8" s="7" t="s">
         <v>33</v>
       </c>
@@ -953,7 +1022,7 @@
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="3:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="12" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="7" t="s">
@@ -973,7 +1042,7 @@
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="3:10" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="10"/>
+      <c r="C10" s="12"/>
       <c r="D10" s="7" t="s">
         <v>56</v>
       </c>
@@ -991,7 +1060,7 @@
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="3:10" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="10"/>
+      <c r="C11" s="12"/>
       <c r="D11" s="7" t="s">
         <v>57</v>
       </c>
@@ -1038,7 +1107,7 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="11" t="s">
         <v>64</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -1052,7 +1121,7 @@
       <c r="B3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="10" t="s">
         <v>67</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1066,7 +1135,7 @@
       <c r="B4" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="10" t="s">
         <v>71</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1080,7 +1149,7 @@
       <c r="B5" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1094,7 +1163,7 @@
       <c r="B6" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="10" t="s">
         <v>74</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1102,6 +1171,174 @@
       </c>
       <c r="E6" s="1" t="s">
         <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:G18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="40.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+    </row>
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+    </row>
+    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D6" s="15"/>
+      <c r="E6" s="14"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" t="s">
+        <v>81</v>
+      </c>
+      <c r="G11" s="16">
+        <v>43232</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12">
+        <v>1074130</v>
+      </c>
+      <c r="D12" s="14">
+        <v>5.3707E-3</v>
+      </c>
+      <c r="E12" s="14">
+        <v>2.98611</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15">
+        <v>68499</v>
+      </c>
+      <c r="D15" s="14">
+        <v>3.4249999999999998E-4</v>
+      </c>
+      <c r="E15" s="14">
+        <v>0.19042999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16">
+        <v>51334</v>
+      </c>
+      <c r="D16" s="14">
+        <v>2.5670000000000001E-4</v>
+      </c>
+      <c r="E16" s="14">
+        <v>0.14273</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17">
+        <v>23034</v>
+      </c>
+      <c r="D17" s="14">
+        <v>1.1519999999999999E-4</v>
+      </c>
+      <c r="E17" s="14">
+        <v>6.4049999999999996E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <f>SUM(C12:C17)</f>
+        <v>1216997</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ref="D18:E18" si="0">SUM(D12:D17)</f>
+        <v>6.0851000000000004E-3</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>3.3833199999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>